<commit_message>
README file committed of 3/9/2022
</commit_message>
<xml_diff>
--- a/manickapremchand_saiprashanthi_capstone_1/documents/Capstone_1_SaiPrashanthiManickaPremchand.xlsx
+++ b/manickapremchand_saiprashanthi_capstone_1/documents/Capstone_1_SaiPrashanthiManickaPremchand.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mppra\PycharmProjects\capstone_1_saiprashanthi_manickapremchand\manickapremchand_saiprashanthi_capstone_1\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F5D330D-C904-4989-8A8E-DCFFC2675857}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D112586-7A29-4237-8B11-3C60A245863E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{05EE201A-0BCA-5646-B296-5AABFBEA194B}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="125">
   <si>
     <t>Functionality</t>
   </si>
@@ -414,13 +414,16 @@
   </si>
   <si>
     <t>Sai Prashanthi Manicka Premchand</t>
+  </si>
+  <si>
+    <t>https://github.com/mpprasanthi/capstone_1_saiprashanthi_manickapremchand.git</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -533,6 +536,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -939,11 +950,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="157">
+  <cellXfs count="158">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1339,8 +1351,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -1664,8 +1680,8 @@
   </sheetPr>
   <dimension ref="B2:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1696,7 +1712,9 @@
       <c r="C5" s="155" t="s">
         <v>117</v>
       </c>
-      <c r="D5" s="153"/>
+      <c r="D5" s="157" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="6" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B6">
@@ -1735,6 +1753,9 @@
       <c r="D9" s="153"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D5" r:id="rId1" xr:uid="{4C93C20E-D8EE-4BE4-ABFF-93DB1B5E44B7}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1746,8 +1767,8 @@
   </sheetPr>
   <dimension ref="A1:W45"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="110" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView zoomScale="110" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2568,26 +2589,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d2a9f884-c2eb-4182-8d97-b2c1069a1e77">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="872877ae-a410-445f-835b-653367d2e530" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FEF7458C51E57141848015B90E19E3FF" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="12fb0db276e8be4984a0823ffe929ad1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d2a9f884-c2eb-4182-8d97-b2c1069a1e77" xmlns:ns3="ad1dcd44-2c79-421e-996d-e07b6b6a06b7" xmlns:ns4="872877ae-a410-445f-835b-653367d2e530" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7f400bb4bb80b6365717ab8834d3c4dc" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="d2a9f884-c2eb-4182-8d97-b2c1069a1e77"/>
@@ -2823,33 +2824,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1DCCBC0B-BA77-41C1-B14F-94133CE8E251}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="ad1dcd44-2c79-421e-996d-e07b6b6a06b7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="d2a9f884-c2eb-4182-8d97-b2c1069a1e77"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="872877ae-a410-445f-835b-653367d2e530"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E8A09A7-4930-415E-BC0E-99BBC8E2BDB5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d2a9f884-c2eb-4182-8d97-b2c1069a1e77">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="872877ae-a410-445f-835b-653367d2e530" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01D904D9-6110-4D51-8C80-718FF126E788}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2867,4 +2862,30 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E8A09A7-4930-415E-BC0E-99BBC8E2BDB5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1DCCBC0B-BA77-41C1-B14F-94133CE8E251}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="ad1dcd44-2c79-421e-996d-e07b6b6a06b7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="d2a9f884-c2eb-4182-8d97-b2c1069a1e77"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="872877ae-a410-445f-835b-653367d2e530"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>